<commit_message>
Working on the revision
</commit_message>
<xml_diff>
--- a/0 Stim/Two Step Stim.xlsx
+++ b/0 Stim/Two Step Stim.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickm\OneDrive\Documents\GitHub\Mediated-Reactivity-2\0 Stim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0061578A-3022-45AF-9D2A-84047F3524C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D74188-E655-464E-9D3F-D2405C7AAABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="11380" windowHeight="13370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="144">
   <si>
     <t>Cue</t>
   </si>
@@ -453,6 +453,21 @@
   </si>
   <si>
     <t>Swab</t>
+  </si>
+  <si>
+    <t>Cue - Med</t>
+  </si>
+  <si>
+    <t>List 1</t>
+  </si>
+  <si>
+    <t>Med -Med</t>
+  </si>
+  <si>
+    <t>Med - Target</t>
+  </si>
+  <si>
+    <t>List 2</t>
   </si>
 </sst>
 </file>
@@ -791,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W39"/>
+  <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2820,7 +2835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="17:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="R34" s="2" t="s">
         <v>0</v>
       </c>
@@ -2832,7 +2847,7 @@
       <c r="V34" s="2"/>
       <c r="W34" s="2"/>
     </row>
-    <row r="35" spans="17:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="R35" s="1" t="s">
         <v>127</v>
       </c>
@@ -2852,7 +2867,21 @@
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="17:23" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F36" s="1"/>
       <c r="Q36" s="1" t="s">
         <v>134</v>
       </c>
@@ -2881,7 +2910,22 @@
         <v>4.3666666666666663</v>
       </c>
     </row>
-    <row r="37" spans="17:23" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="B37" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37">
+        <f>AVERAGE(E3:E17)</f>
+        <v>0.29086666666666666</v>
+      </c>
+      <c r="D37">
+        <f>AVERAGE(I3:I17)</f>
+        <v>0.112</v>
+      </c>
+      <c r="E37">
+        <f>AVERAGE(M3:M17)</f>
+        <v>0.1970666666666667</v>
+      </c>
       <c r="Q37" s="1" t="s">
         <v>135</v>
       </c>
@@ -2910,7 +2954,22 @@
         <v>1.1591713250937246</v>
       </c>
     </row>
-    <row r="38" spans="17:23" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="B38" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C38">
+        <f>STDEV(E3:E17)</f>
+        <v>0.23784114346304666</v>
+      </c>
+      <c r="D38">
+        <f>STDEV(F3:I17)</f>
+        <v>0.13012576334344514</v>
+      </c>
+      <c r="E38">
+        <f>STDEV(M3:M17)</f>
+        <v>0.11981143915495272</v>
+      </c>
       <c r="Q38" s="1" t="s">
         <v>136</v>
       </c>
@@ -2939,7 +2998,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="17:23" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="B39" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C39">
+        <f>MIN(E3:E17)</f>
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <f>MIN(I3:I17)</f>
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <f>MIN(M3:M17)</f>
+        <v>7.9000000000000001E-2</v>
+      </c>
       <c r="Q39" s="1" t="s">
         <v>137</v>
       </c>
@@ -2966,6 +3040,106 @@
       <c r="W39">
         <f t="shared" si="5"/>
         <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="B40" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C40">
+        <f>MAX(E3:E17)</f>
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="D40">
+        <f>MAX(I3:I17)</f>
+        <v>0.44</v>
+      </c>
+      <c r="E40">
+        <f>MAX(M3:M17)</f>
+        <v>0.503</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="B43" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43">
+        <f>AVERAGE(E18:E32)</f>
+        <v>0.16899999999999998</v>
+      </c>
+      <c r="D43">
+        <f>AVERAGE(I18:I32)</f>
+        <v>6.660000000000002E-2</v>
+      </c>
+      <c r="E43">
+        <f>AVERAGE(M18:M32)</f>
+        <v>0.22446666666666668</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="B44" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44">
+        <f>STDEV(E18:E32)</f>
+        <v>0.15336976792799067</v>
+      </c>
+      <c r="D44">
+        <f>STDEV(F18:I32)</f>
+        <v>6.3738080118111939E-2</v>
+      </c>
+      <c r="E44">
+        <f>STDEV(M18:M32)</f>
+        <v>0.13021019636762413</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="B45" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C45">
+        <f>MIN(E18:E32)</f>
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <f>MIN(I18:I32)</f>
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <f>MIN(M18:M32)</f>
+        <v>8.6999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="B46" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C46">
+        <f>MAX(E18:E32)</f>
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="D46">
+        <f>MAX(I18:I32)</f>
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="E46">
+        <f>MAX(M18:M32)</f>
+        <v>0.51800000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>